<commit_message>
poster creation & sound recordings
</commit_message>
<xml_diff>
--- a/New Idea/Planner.xlsx
+++ b/New Idea/Planner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukeh\Desktop\Dissertation\New Idea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2A49E3-0DBE-48B1-B1DF-53E8B1B1F578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EA7F18-E80E-459C-9B9F-282B61BF6BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4F1C073E-7DB9-E242-BB39-302AFDA3FEA0}"/>
   </bookViews>
@@ -429,9 +429,6 @@
     <t>Start designing poster</t>
   </si>
   <si>
-    <t>Start poster presentation</t>
-  </si>
-  <si>
     <t>User testing</t>
   </si>
   <si>
@@ -478,6 +475,9 @@
   </si>
   <si>
     <t xml:space="preserve">18th Jan Poster Submission      </t>
+  </si>
+  <si>
+    <t>Start poster</t>
   </si>
 </sst>
 </file>
@@ -909,6 +909,27 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -929,27 +950,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1316,34 +1316,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="43"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" ht="57.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="37" t="s">
+      <c r="B2" s="45"/>
+      <c r="C2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="38" t="s">
+      <c r="D2" s="46"/>
+      <c r="E2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="39"/>
-      <c r="G2" s="37" t="s">
+      <c r="F2" s="46"/>
+      <c r="G2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="39"/>
+      <c r="H2" s="46"/>
     </row>
     <row r="3" spans="1:8" ht="90.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1482,14 +1482,14 @@
       <c r="B12" s="18">
         <v>45211</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="44" t="s">
+      <c r="C12" s="41"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="45"/>
+      <c r="H12" s="38"/>
     </row>
     <row r="13" spans="1:8" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
@@ -1498,14 +1498,14 @@
       <c r="B13" s="19">
         <v>45225</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="46" t="s">
+      <c r="C13" s="42"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="47"/>
+      <c r="H13" s="40"/>
     </row>
     <row r="14" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
@@ -1607,17 +1607,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A1:H1"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1628,7 +1628,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1814,13 +1814,13 @@
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E10" s="22">
         <v>100</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G10" s="22">
         <v>100</v>
@@ -1838,13 +1838,13 @@
         <v>87</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E11" s="22">
         <v>100</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G11" s="22">
         <v>100</v>
@@ -1860,7 +1860,7 @@
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E12" s="22">
         <v>100</v>
@@ -1882,13 +1882,13 @@
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E13" s="22">
         <v>100</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G13" s="22">
         <v>100</v>
@@ -1907,10 +1907,10 @@
         <v>129</v>
       </c>
       <c r="E14" s="22">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G14" s="22">
         <v>100</v>
@@ -1926,14 +1926,16 @@
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E15" s="22">
+        <v>80</v>
+      </c>
+      <c r="F15" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="21" t="s">
-        <v>131</v>
-      </c>
       <c r="G15" s="22">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="H15" s="21"/>
     </row>
@@ -1945,14 +1947,14 @@
         <v>65</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>101</v>
       </c>
       <c r="E16" s="22"/>
       <c r="F16" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="21"/>
@@ -1968,11 +1970,11 @@
         <v>100</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="21"/>
@@ -1986,11 +1988,11 @@
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="21"/>
@@ -2004,7 +2006,7 @@
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="21"/>
@@ -2020,7 +2022,7 @@
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="21"/>
@@ -2036,11 +2038,11 @@
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E21" s="22"/>
       <c r="F21" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="21"/>
@@ -2058,7 +2060,7 @@
       </c>
       <c r="E22" s="22"/>
       <c r="F22" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G22" s="22"/>
       <c r="H22" s="21"/>
@@ -2072,11 +2074,11 @@
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E23" s="22"/>
       <c r="F23" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="21"/>
@@ -2090,11 +2092,11 @@
       </c>
       <c r="C24" s="31"/>
       <c r="D24" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E24" s="32"/>
       <c r="F24" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G24" s="32"/>
       <c r="H24" s="31"/>

</xml_diff>